<commit_message>
Add proto output functions
</commit_message>
<xml_diff>
--- a/test/Sample.xlsx
+++ b/test/Sample.xlsx
@@ -18,54 +18,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="53">
   <si>
     <t>required</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>optional</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>optional</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>repeated</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>optional_struct</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>uint64</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>int64</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>string</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>SampleID</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Times</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>NameID</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>uint32</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -81,7 +81,7 @@
       </rPr>
       <t>omment1</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -97,15 +97,15 @@
       </rPr>
       <t>xtra Comments</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Comment2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Comment3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -121,7 +121,7 @@
       </rPr>
       <t>tructName</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -137,7 +137,7 @@
       </rPr>
       <t>ewardID</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -153,7 +153,7 @@
       </rPr>
       <t>ount</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -169,7 +169,7 @@
       </rPr>
       <t>eight</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -185,7 +185,7 @@
       </rPr>
       <t>omment4</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -201,7 +201,7 @@
       </rPr>
       <t>omment5</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -217,7 +217,7 @@
       </rPr>
       <t>omment6</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -233,15 +233,15 @@
       </rPr>
       <t>64</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>SAMPLEONE contains right data</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>SAMPLETWO contains incorrect data</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -257,11 +257,11 @@
       </rPr>
       <t>oo?</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Name1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -277,7 +277,7 @@
       </rPr>
       <t>tem1</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -293,7 +293,7 @@
       </rPr>
       <t>tem2</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -309,11 +309,11 @@
       </rPr>
       <t>tem3</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Name2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Name3</t>
@@ -348,27 +348,27 @@
       </rPr>
       <t>titles</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Item4</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>repeat value -</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>repeat value +</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>repeat value overflow</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>value type incorrect</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -384,11 +384,11 @@
       </rPr>
       <t>d001</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>value incorrect</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -404,7 +404,7 @@
       </rPr>
       <t>one</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -420,7 +420,7 @@
       </rPr>
       <t>s</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -436,7 +436,7 @@
       </rPr>
       <t>e</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -452,7 +452,7 @@
       </rPr>
       <t>64</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -468,36 +468,47 @@
       </rPr>
       <t>FOUR has same structure with SAMPLEONE but different ID</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>optional</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>repeated</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>optional_struct</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>required</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProtoVarName</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -587,19 +598,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -938,7 +950,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1304,7 +1316,7 @@
       <c r="O9" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1764,7 +1776,7 @@
       <c r="S9" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2141,7 +2153,7 @@
       <c r="P9" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2152,7 +2164,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2330,6 +2342,9 @@
       <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="F4" s="14" t="s">
+        <v>52</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>20</v>
       </c>
@@ -2339,6 +2354,9 @@
       <c r="I4" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="J4" s="14" t="s">
+        <v>52</v>
+      </c>
       <c r="K4" s="2" t="s">
         <v>20</v>
       </c>
@@ -2347,6 +2365,9 @@
       </c>
       <c r="M4" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>20</v>
@@ -2507,7 +2528,7 @@
       <c r="O9" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add functions to encode xlsx data
</commit_message>
<xml_diff>
--- a/test/Sample.xlsx
+++ b/test/Sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -18,54 +18,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="65">
   <si>
     <t>required</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>optional</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>optional</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>repeated</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>optional_struct</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>uint64</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>int64</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>string</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>SampleID</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Times</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>NameID</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>uint32</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -81,7 +81,7 @@
       </rPr>
       <t>omment1</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -97,15 +97,15 @@
       </rPr>
       <t>xtra Comments</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Comment2</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Comment3</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -121,7 +121,7 @@
       </rPr>
       <t>tructName</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -137,7 +137,7 @@
       </rPr>
       <t>ewardID</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -153,7 +153,7 @@
       </rPr>
       <t>ount</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -169,7 +169,7 @@
       </rPr>
       <t>eight</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -185,7 +185,7 @@
       </rPr>
       <t>omment4</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -201,7 +201,7 @@
       </rPr>
       <t>omment5</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -217,7 +217,7 @@
       </rPr>
       <t>omment6</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -233,15 +233,15 @@
       </rPr>
       <t>64</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>SAMPLEONE contains right data</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>SAMPLETWO contains incorrect data</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -257,11 +257,11 @@
       </rPr>
       <t>oo?</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Name1</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -277,7 +277,7 @@
       </rPr>
       <t>tem1</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -293,7 +293,7 @@
       </rPr>
       <t>tem2</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -309,11 +309,11 @@
       </rPr>
       <t>tem3</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Name2</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Name3</t>
@@ -348,27 +348,27 @@
       </rPr>
       <t>titles</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Item4</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>repeat value -</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>repeat value +</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>repeat value overflow</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>value type incorrect</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -384,11 +384,11 @@
       </rPr>
       <t>d001</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>value incorrect</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -404,7 +404,7 @@
       </rPr>
       <t>one</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -420,7 +420,7 @@
       </rPr>
       <t>s</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -436,7 +436,7 @@
       </rPr>
       <t>e</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -452,7 +452,7 @@
       </rPr>
       <t>64</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -468,40 +468,102 @@
       </rPr>
       <t>FOUR has same structure with SAMPLEONE but different ID</t>
     </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>optional</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>repeated</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>optional_struct</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>required</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>ProtoVarName</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>御坂美琴</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>白井黑子</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>初春饰利</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>佐天泪子</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>食蜂 操祈</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEVEL5</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>常盘台中学</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>第三位</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEVEL4</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>177支部所属风纪委员</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEVEL1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -598,19 +660,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -950,7 +1014,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -960,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A1:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -973,7 +1037,8 @@
     <col min="6" max="6" width="13.75" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="10.625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.75" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="10.625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="9" style="1"/>
@@ -1177,14 +1242,14 @@
       <c r="C5" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>27</v>
+      <c r="D5" s="16" t="s">
+        <v>54</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>28</v>
+      <c r="G5" s="16" t="s">
+        <v>59</v>
       </c>
       <c r="H5" s="1">
         <v>25</v>
@@ -1192,8 +1257,8 @@
       <c r="I5" s="1">
         <v>0.2</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>29</v>
+      <c r="K5" s="16" t="s">
+        <v>60</v>
       </c>
       <c r="L5" s="1">
         <v>30</v>
@@ -1201,8 +1266,8 @@
       <c r="M5" s="1">
         <v>0.3</v>
       </c>
-      <c r="O5" s="3" t="s">
-        <v>30</v>
+      <c r="O5" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="P5" s="1">
         <v>50</v>
@@ -1221,26 +1286,26 @@
       <c r="C6" s="1">
         <v>6</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>31</v>
+      <c r="D6" s="16" t="s">
+        <v>55</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>28</v>
+      <c r="G6" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="H6" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I6" s="1">
         <v>0.4</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>29</v>
+      <c r="K6" s="16" t="s">
+        <v>63</v>
       </c>
       <c r="L6" s="1">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="M6" s="1">
         <v>0.6</v>
@@ -1257,17 +1322,17 @@
       <c r="C7" s="1">
         <v>9</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>32</v>
+      <c r="D7" s="16" t="s">
+        <v>56</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>28</v>
+      <c r="G7" s="16" t="s">
+        <v>64</v>
       </c>
       <c r="H7" s="1">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I7" s="1">
         <v>1</v>
@@ -1285,8 +1350,8 @@
       <c r="C8" s="1">
         <v>18</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>33</v>
+      <c r="D8" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
@@ -1305,8 +1370,8 @@
       <c r="C9" s="1">
         <v>43</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>34</v>
+      <c r="D9" s="16" t="s">
+        <v>58</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -1316,7 +1381,7 @@
       <c r="O9" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1776,7 +1841,7 @@
       <c r="S9" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2153,7 +2218,7 @@
       <c r="P9" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2163,8 +2228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2254,8 +2319,8 @@
       <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>23</v>
+      <c r="I2" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="J2" s="1">
         <v>3</v>
@@ -2266,8 +2331,8 @@
       <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>23</v>
+      <c r="M2" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="N2" s="1">
         <v>3</v>
@@ -2278,8 +2343,8 @@
       <c r="P2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>23</v>
+      <c r="Q2" s="15" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -2528,7 +2593,7 @@
       <c r="O9" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>